<commit_message>
ẩn ví dụ bổ sung
</commit_message>
<xml_diff>
--- a/public/KANJI_N3.xlsx
+++ b/public/KANJI_N3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chiba\Desktop\Japanese\kanji\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B394C37B-7B72-4CF9-B1A3-55E4DCBD09A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F478BAAB-863D-47DA-8B4F-2D21ABC733BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,28 +39,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -65279,10 +65257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H1612"/>
+  <dimension ref="A1:H1613"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
+    <sheetView tabSelected="1" topLeftCell="A1547" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E1552" sqref="E1552"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -90552,55 +90530,51 @@
       <c r="G1552" s="3"/>
       <c r="H1552" s="3"/>
     </row>
-    <row r="1553" spans="1:8">
-      <c r="A1553" cm="1">
-        <f t="array" ref="A1553">SUMPRODUCT(LEN(A2:A1550))</f>
-        <v>832</v>
-      </c>
+    <row r="1553" spans="2:8">
       <c r="B1553" s="3"/>
       <c r="E1553" s="3"/>
       <c r="F1553" s="3"/>
       <c r="G1553" s="3"/>
       <c r="H1553" s="3"/>
     </row>
-    <row r="1554" spans="1:8">
+    <row r="1554" spans="2:8">
       <c r="B1554" s="3"/>
       <c r="E1554" s="3"/>
       <c r="F1554" s="3"/>
       <c r="G1554" s="3"/>
       <c r="H1554" s="3"/>
     </row>
-    <row r="1555" spans="1:8">
+    <row r="1555" spans="2:8">
       <c r="B1555" s="3"/>
       <c r="E1555" s="3"/>
       <c r="F1555" s="3"/>
       <c r="G1555" s="3"/>
       <c r="H1555" s="3"/>
     </row>
-    <row r="1556" spans="1:8">
+    <row r="1556" spans="2:8">
       <c r="B1556" s="3"/>
       <c r="E1556" s="3"/>
       <c r="F1556" s="3"/>
       <c r="G1556" s="3"/>
       <c r="H1556" s="3"/>
     </row>
-    <row r="1557" spans="1:8" ht="27">
+    <row r="1557" spans="2:8" ht="27">
       <c r="E1557" ph="1"/>
       <c r="F1557" ph="1"/>
     </row>
-    <row r="1560" spans="1:8" ht="27">
+    <row r="1560" spans="2:8" ht="27">
       <c r="E1560" ph="1"/>
       <c r="F1560" ph="1"/>
     </row>
-    <row r="1565" spans="1:8" ht="27">
+    <row r="1565" spans="2:8" ht="27">
       <c r="E1565" ph="1"/>
       <c r="F1565" ph="1"/>
     </row>
-    <row r="1566" spans="1:8" ht="27">
+    <row r="1566" spans="2:8" ht="27">
       <c r="E1566" ph="1"/>
       <c r="F1566" ph="1"/>
     </row>
-    <row r="1567" spans="1:8" ht="27">
+    <row r="1567" spans="2:8" ht="27">
       <c r="E1567" ph="1"/>
       <c r="F1567" ph="1"/>
     </row>
@@ -90751,6 +90725,10 @@
     <row r="1612" spans="5:6" ht="27">
       <c r="E1612" ph="1"/>
       <c r="F1612" ph="1"/>
+    </row>
+    <row r="1613" spans="5:6" ht="27">
+      <c r="E1613" ph="1"/>
+      <c r="F1613" ph="1"/>
     </row>
   </sheetData>
   <mergeCells count="1940">
@@ -90812,6 +90790,12 @@
     <mergeCell ref="A425:A426"/>
     <mergeCell ref="A423:A424"/>
     <mergeCell ref="A249:A250"/>
+    <mergeCell ref="D878:D879"/>
+    <mergeCell ref="C878:C879"/>
+    <mergeCell ref="B878:B879"/>
+    <mergeCell ref="A878:A879"/>
+    <mergeCell ref="D356:D357"/>
+    <mergeCell ref="A394:A397"/>
     <mergeCell ref="D147:D148"/>
     <mergeCell ref="C147:C148"/>
     <mergeCell ref="B147:B148"/>
@@ -90829,10 +90813,6 @@
     <mergeCell ref="C416:C417"/>
     <mergeCell ref="D416:D417"/>
     <mergeCell ref="D407:D409"/>
-    <mergeCell ref="D878:D879"/>
-    <mergeCell ref="C878:C879"/>
-    <mergeCell ref="B878:B879"/>
-    <mergeCell ref="A878:A879"/>
     <mergeCell ref="A430:A431"/>
     <mergeCell ref="A427:A429"/>
     <mergeCell ref="B430:B431"/>
@@ -90848,42 +90828,6 @@
     <mergeCell ref="A356:A357"/>
     <mergeCell ref="B356:B357"/>
     <mergeCell ref="C356:C357"/>
-    <mergeCell ref="D356:D357"/>
-    <mergeCell ref="A394:A397"/>
-    <mergeCell ref="B394:B397"/>
-    <mergeCell ref="C394:C397"/>
-    <mergeCell ref="D394:D397"/>
-    <mergeCell ref="A391:A392"/>
-    <mergeCell ref="B391:B392"/>
-    <mergeCell ref="C391:C392"/>
-    <mergeCell ref="D391:D392"/>
-    <mergeCell ref="A383:A385"/>
-    <mergeCell ref="B383:B385"/>
-    <mergeCell ref="C383:C385"/>
-    <mergeCell ref="D383:D385"/>
-    <mergeCell ref="A364:A367"/>
-    <mergeCell ref="A380:A381"/>
-    <mergeCell ref="B380:B381"/>
-    <mergeCell ref="C380:C381"/>
-    <mergeCell ref="D380:D381"/>
-    <mergeCell ref="C362:C363"/>
-    <mergeCell ref="B362:B363"/>
-    <mergeCell ref="A362:A363"/>
-    <mergeCell ref="A360:A361"/>
-    <mergeCell ref="B360:B361"/>
-    <mergeCell ref="C360:C361"/>
-    <mergeCell ref="D360:D361"/>
-    <mergeCell ref="D371:D372"/>
-    <mergeCell ref="C371:C372"/>
-    <mergeCell ref="B371:B372"/>
-    <mergeCell ref="A371:A372"/>
-    <mergeCell ref="D358:D359"/>
-    <mergeCell ref="C358:C359"/>
-    <mergeCell ref="B358:B359"/>
-    <mergeCell ref="A358:A359"/>
-    <mergeCell ref="A420:A422"/>
-    <mergeCell ref="B420:B422"/>
-    <mergeCell ref="C420:C422"/>
     <mergeCell ref="D420:D422"/>
     <mergeCell ref="B412:B414"/>
     <mergeCell ref="A412:A414"/>
@@ -90901,14 +90845,21 @@
     <mergeCell ref="C410:C411"/>
     <mergeCell ref="B410:B411"/>
     <mergeCell ref="A410:A411"/>
-    <mergeCell ref="A416:A417"/>
-    <mergeCell ref="B364:B367"/>
-    <mergeCell ref="C364:C367"/>
-    <mergeCell ref="D364:D367"/>
-    <mergeCell ref="D388:D389"/>
-    <mergeCell ref="C418:C419"/>
-    <mergeCell ref="D418:D419"/>
-    <mergeCell ref="B418:B419"/>
+    <mergeCell ref="B394:B397"/>
+    <mergeCell ref="C394:C397"/>
+    <mergeCell ref="D394:D397"/>
+    <mergeCell ref="A391:A392"/>
+    <mergeCell ref="B391:B392"/>
+    <mergeCell ref="C391:C392"/>
+    <mergeCell ref="D391:D392"/>
+    <mergeCell ref="A383:A385"/>
+    <mergeCell ref="B383:B385"/>
+    <mergeCell ref="C383:C385"/>
+    <mergeCell ref="D383:D385"/>
+    <mergeCell ref="A380:A381"/>
+    <mergeCell ref="B380:B381"/>
+    <mergeCell ref="C380:C381"/>
+    <mergeCell ref="D380:D381"/>
     <mergeCell ref="A351:A353"/>
     <mergeCell ref="B351:B353"/>
     <mergeCell ref="C351:C353"/>
@@ -90921,6 +90872,22 @@
     <mergeCell ref="B346:B347"/>
     <mergeCell ref="C346:C347"/>
     <mergeCell ref="D346:D347"/>
+    <mergeCell ref="A360:A361"/>
+    <mergeCell ref="B360:B361"/>
+    <mergeCell ref="C360:C361"/>
+    <mergeCell ref="D360:D361"/>
+    <mergeCell ref="D371:D372"/>
+    <mergeCell ref="C371:C372"/>
+    <mergeCell ref="B371:B372"/>
+    <mergeCell ref="A371:A372"/>
+    <mergeCell ref="D358:D359"/>
+    <mergeCell ref="C358:C359"/>
+    <mergeCell ref="B358:B359"/>
+    <mergeCell ref="A358:A359"/>
+    <mergeCell ref="A364:A367"/>
+    <mergeCell ref="C362:C363"/>
+    <mergeCell ref="B362:B363"/>
+    <mergeCell ref="A362:A363"/>
     <mergeCell ref="C442:C443"/>
     <mergeCell ref="B442:B443"/>
     <mergeCell ref="A442:A443"/>
@@ -90941,6 +90908,18 @@
     <mergeCell ref="C437:C438"/>
     <mergeCell ref="B437:B438"/>
     <mergeCell ref="A437:A438"/>
+    <mergeCell ref="D442:D443"/>
+    <mergeCell ref="A416:A417"/>
+    <mergeCell ref="B364:B367"/>
+    <mergeCell ref="C364:C367"/>
+    <mergeCell ref="D364:D367"/>
+    <mergeCell ref="D388:D389"/>
+    <mergeCell ref="C418:C419"/>
+    <mergeCell ref="D418:D419"/>
+    <mergeCell ref="B418:B419"/>
+    <mergeCell ref="A420:A422"/>
+    <mergeCell ref="B420:B422"/>
+    <mergeCell ref="C420:C422"/>
     <mergeCell ref="D344:D345"/>
     <mergeCell ref="C344:C345"/>
     <mergeCell ref="B344:B345"/>
@@ -91041,9 +91020,6 @@
     <mergeCell ref="C284:C286"/>
     <mergeCell ref="B284:B286"/>
     <mergeCell ref="A284:A286"/>
-    <mergeCell ref="A251:A253"/>
-    <mergeCell ref="B251:B253"/>
-    <mergeCell ref="C251:C253"/>
     <mergeCell ref="D251:D253"/>
     <mergeCell ref="D215:D216"/>
     <mergeCell ref="C215:C216"/>
@@ -91296,6 +91272,11 @@
     <mergeCell ref="B125:B126"/>
     <mergeCell ref="C125:C126"/>
     <mergeCell ref="D125:D126"/>
+    <mergeCell ref="D468:D470"/>
+    <mergeCell ref="D464:D465"/>
+    <mergeCell ref="C462:C463"/>
+    <mergeCell ref="B462:B463"/>
+    <mergeCell ref="A462:A463"/>
     <mergeCell ref="B165:B167"/>
     <mergeCell ref="D165:D167"/>
     <mergeCell ref="C165:C167"/>
@@ -91320,6 +91301,14 @@
     <mergeCell ref="C171:C172"/>
     <mergeCell ref="B171:B172"/>
     <mergeCell ref="A171:A172"/>
+    <mergeCell ref="A251:A253"/>
+    <mergeCell ref="B251:B253"/>
+    <mergeCell ref="C251:C253"/>
+    <mergeCell ref="C507:C508"/>
+    <mergeCell ref="D507:D508"/>
+    <mergeCell ref="D509:D510"/>
+    <mergeCell ref="C509:C510"/>
+    <mergeCell ref="B509:B510"/>
     <mergeCell ref="D188:D189"/>
     <mergeCell ref="C188:C189"/>
     <mergeCell ref="B188:B189"/>
@@ -91347,41 +91336,6 @@
     <mergeCell ref="A474:A475"/>
     <mergeCell ref="C466:C467"/>
     <mergeCell ref="D466:D467"/>
-    <mergeCell ref="D468:D470"/>
-    <mergeCell ref="D464:D465"/>
-    <mergeCell ref="C462:C463"/>
-    <mergeCell ref="B462:B463"/>
-    <mergeCell ref="A462:A463"/>
-    <mergeCell ref="D500:D501"/>
-    <mergeCell ref="D485:D487"/>
-    <mergeCell ref="C485:C487"/>
-    <mergeCell ref="B485:B487"/>
-    <mergeCell ref="A485:A487"/>
-    <mergeCell ref="A488:A489"/>
-    <mergeCell ref="D494:D496"/>
-    <mergeCell ref="C494:C496"/>
-    <mergeCell ref="B494:B496"/>
-    <mergeCell ref="A494:A496"/>
-    <mergeCell ref="A507:A508"/>
-    <mergeCell ref="B507:B508"/>
-    <mergeCell ref="C507:C508"/>
-    <mergeCell ref="D507:D508"/>
-    <mergeCell ref="D509:D510"/>
-    <mergeCell ref="C509:C510"/>
-    <mergeCell ref="B509:B510"/>
-    <mergeCell ref="D442:D443"/>
-    <mergeCell ref="B466:B467"/>
-    <mergeCell ref="A466:A467"/>
-    <mergeCell ref="A464:A465"/>
-    <mergeCell ref="B464:B465"/>
-    <mergeCell ref="C464:C465"/>
-    <mergeCell ref="D450:D451"/>
-    <mergeCell ref="C450:C451"/>
-    <mergeCell ref="B450:B451"/>
-    <mergeCell ref="A450:A451"/>
-    <mergeCell ref="A448:A449"/>
-    <mergeCell ref="B448:B449"/>
-    <mergeCell ref="C448:C449"/>
     <mergeCell ref="D448:D449"/>
     <mergeCell ref="B468:B470"/>
     <mergeCell ref="C468:C470"/>
@@ -91399,6 +91353,21 @@
     <mergeCell ref="B488:B489"/>
     <mergeCell ref="C488:C489"/>
     <mergeCell ref="D488:D489"/>
+    <mergeCell ref="C533:C534"/>
+    <mergeCell ref="B533:B534"/>
+    <mergeCell ref="A533:A534"/>
+    <mergeCell ref="D500:D501"/>
+    <mergeCell ref="D485:D487"/>
+    <mergeCell ref="C485:C487"/>
+    <mergeCell ref="B485:B487"/>
+    <mergeCell ref="A485:A487"/>
+    <mergeCell ref="A488:A489"/>
+    <mergeCell ref="D494:D496"/>
+    <mergeCell ref="C494:C496"/>
+    <mergeCell ref="B494:B496"/>
+    <mergeCell ref="A494:A496"/>
+    <mergeCell ref="A507:A508"/>
+    <mergeCell ref="B507:B508"/>
     <mergeCell ref="A445:A447"/>
     <mergeCell ref="B445:B447"/>
     <mergeCell ref="C445:C447"/>
@@ -91419,9 +91388,18 @@
     <mergeCell ref="C502:C503"/>
     <mergeCell ref="D502:D503"/>
     <mergeCell ref="A509:A510"/>
-    <mergeCell ref="C533:C534"/>
-    <mergeCell ref="B533:B534"/>
-    <mergeCell ref="A533:A534"/>
+    <mergeCell ref="B466:B467"/>
+    <mergeCell ref="A466:A467"/>
+    <mergeCell ref="A464:A465"/>
+    <mergeCell ref="B464:B465"/>
+    <mergeCell ref="C464:C465"/>
+    <mergeCell ref="D450:D451"/>
+    <mergeCell ref="C450:C451"/>
+    <mergeCell ref="B450:B451"/>
+    <mergeCell ref="A450:A451"/>
+    <mergeCell ref="A448:A449"/>
+    <mergeCell ref="B448:B449"/>
+    <mergeCell ref="C448:C449"/>
     <mergeCell ref="A531:A532"/>
     <mergeCell ref="B531:B532"/>
     <mergeCell ref="C531:C532"/>

</xml_diff>